<commit_message>
Added simd2012 data file
</commit_message>
<xml_diff>
--- a/opengov/sds2011.xlsx
+++ b/opengov/sds2011.xlsx
@@ -794,10 +794,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1051,7 +1065,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="69">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1079,6 +1093,13 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1105,6 +1126,13 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -3324,10 +3352,10 @@
   <dimension ref="A1:BM54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE46" sqref="AE46"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added prevalence over time into spreadsheet
</commit_message>
<xml_diff>
--- a/opengov/sds2011.xlsx
+++ b/opengov/sds2011.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="560" windowWidth="25040" windowHeight="14140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="prevelence" sheetId="19" r:id="rId1"/>
-    <sheet name="fact" sheetId="14" r:id="rId2"/>
-    <sheet name="summarymatrix" sheetId="11" r:id="rId3"/>
+    <sheet name="prevelence_by_year" sheetId="20" r:id="rId2"/>
+    <sheet name="fact" sheetId="14" r:id="rId3"/>
+    <sheet name="summary_matrix" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fact!$A$1:$C$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">fact!$A$1:$C$155</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="183">
   <si>
     <t>metric</t>
   </si>
@@ -567,6 +568,12 @@
   </si>
   <si>
     <t>% of diabetes pop with HbA1c recorded</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>midyrpe</t>
   </si>
 </sst>
 </file>
@@ -893,7 +900,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,6 +1106,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="91">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1491,7 +1499,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2100,10 +2108,1450 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="101" customFormat="1">
+      <c r="A1" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="101" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="101" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="101" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <v>2011</v>
+      </c>
+      <c r="C2">
+        <v>2221</v>
+      </c>
+      <c r="D2">
+        <v>17919</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>366860</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>2011</v>
+      </c>
+      <c r="C3">
+        <v>614</v>
+      </c>
+      <c r="D3">
+        <v>4846</v>
+      </c>
+      <c r="E3">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>112870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>2011</v>
+      </c>
+      <c r="C4">
+        <v>893</v>
+      </c>
+      <c r="D4">
+        <v>7236</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+      <c r="F4">
+        <v>148190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5">
+        <v>1969</v>
+      </c>
+      <c r="D5">
+        <v>16164</v>
+      </c>
+      <c r="E5">
+        <v>59</v>
+      </c>
+      <c r="F5">
+        <v>364945</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <v>2011</v>
+      </c>
+      <c r="C6">
+        <v>1606</v>
+      </c>
+      <c r="D6">
+        <v>12528</v>
+      </c>
+      <c r="E6">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>293386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>2011</v>
+      </c>
+      <c r="C7">
+        <v>3053</v>
+      </c>
+      <c r="D7">
+        <v>20902</v>
+      </c>
+      <c r="E7">
+        <v>85</v>
+      </c>
+      <c r="F7">
+        <v>550620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>2011</v>
+      </c>
+      <c r="C8">
+        <v>6180</v>
+      </c>
+      <c r="D8">
+        <v>50005</v>
+      </c>
+      <c r="E8">
+        <v>527</v>
+      </c>
+      <c r="F8">
+        <v>1203870</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <v>2011</v>
+      </c>
+      <c r="C9">
+        <v>1758</v>
+      </c>
+      <c r="D9">
+        <v>12479</v>
+      </c>
+      <c r="E9">
+        <v>128</v>
+      </c>
+      <c r="F9">
+        <v>310830</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10">
+        <v>2011</v>
+      </c>
+      <c r="C10">
+        <v>3513</v>
+      </c>
+      <c r="D10">
+        <v>24998</v>
+      </c>
+      <c r="E10">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>562477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11">
+        <v>2011</v>
+      </c>
+      <c r="C11">
+        <v>4175</v>
+      </c>
+      <c r="D11">
+        <v>29551</v>
+      </c>
+      <c r="E11">
+        <v>298</v>
+      </c>
+      <c r="F11">
+        <v>836711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12">
+        <v>2011</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="D12">
+        <v>853</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>20110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>2011</v>
+      </c>
+      <c r="C13">
+        <v>124</v>
+      </c>
+      <c r="D13">
+        <v>871</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>22400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14">
+        <v>2011</v>
+      </c>
+      <c r="C14">
+        <v>1864</v>
+      </c>
+      <c r="D14">
+        <v>18104</v>
+      </c>
+      <c r="E14">
+        <v>98</v>
+      </c>
+      <c r="F14">
+        <v>402641</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15">
+        <v>2011</v>
+      </c>
+      <c r="C15">
+        <v>182</v>
+      </c>
+      <c r="D15">
+        <v>1058</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>26190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>2010</v>
+      </c>
+      <c r="C16">
+        <v>2238</v>
+      </c>
+      <c r="D16">
+        <v>16775</v>
+      </c>
+      <c r="E16">
+        <v>62</v>
+      </c>
+      <c r="F16">
+        <v>367160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>2010</v>
+      </c>
+      <c r="C17">
+        <v>601</v>
+      </c>
+      <c r="D17">
+        <v>4728</v>
+      </c>
+      <c r="E17">
+        <v>26</v>
+      </c>
+      <c r="F17">
+        <v>112680</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>2010</v>
+      </c>
+      <c r="C18">
+        <v>888</v>
+      </c>
+      <c r="D18">
+        <v>6836</v>
+      </c>
+      <c r="E18">
+        <v>47</v>
+      </c>
+      <c r="F18">
+        <v>148510</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>2010</v>
+      </c>
+      <c r="C19">
+        <v>1911</v>
+      </c>
+      <c r="D19">
+        <v>15480</v>
+      </c>
+      <c r="E19">
+        <v>76</v>
+      </c>
+      <c r="F19">
+        <v>363385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20">
+        <v>2010</v>
+      </c>
+      <c r="C20">
+        <v>1568</v>
+      </c>
+      <c r="D20">
+        <v>12007</v>
+      </c>
+      <c r="E20">
+        <v>43</v>
+      </c>
+      <c r="F20">
+        <v>291383</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>2010</v>
+      </c>
+      <c r="C21">
+        <v>3045</v>
+      </c>
+      <c r="D21">
+        <v>20227</v>
+      </c>
+      <c r="E21">
+        <v>85</v>
+      </c>
+      <c r="F21">
+        <v>544980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22">
+        <v>2010</v>
+      </c>
+      <c r="C22">
+        <v>6115</v>
+      </c>
+      <c r="D22">
+        <v>48090</v>
+      </c>
+      <c r="E22">
+        <v>265</v>
+      </c>
+      <c r="F22">
+        <v>1199026</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>2010</v>
+      </c>
+      <c r="C23">
+        <v>1706</v>
+      </c>
+      <c r="D23">
+        <v>12100</v>
+      </c>
+      <c r="E23">
+        <v>108</v>
+      </c>
+      <c r="F23">
+        <v>310530</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24">
+        <v>2010</v>
+      </c>
+      <c r="C24">
+        <v>3480</v>
+      </c>
+      <c r="D24">
+        <v>23840</v>
+      </c>
+      <c r="E24">
+        <v>130</v>
+      </c>
+      <c r="F24">
+        <v>562215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <v>2010</v>
+      </c>
+      <c r="C25">
+        <v>4109</v>
+      </c>
+      <c r="D25">
+        <v>28279</v>
+      </c>
+      <c r="E25">
+        <v>329</v>
+      </c>
+      <c r="F25">
+        <v>826231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26">
+        <v>2010</v>
+      </c>
+      <c r="C26">
+        <v>116</v>
+      </c>
+      <c r="D26">
+        <v>807</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>19960</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27">
+        <v>2010</v>
+      </c>
+      <c r="C27">
+        <v>119</v>
+      </c>
+      <c r="D27">
+        <v>834</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>22210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28">
+        <v>2010</v>
+      </c>
+      <c r="C28">
+        <v>1837</v>
+      </c>
+      <c r="D28">
+        <v>17283</v>
+      </c>
+      <c r="E28">
+        <v>103</v>
+      </c>
+      <c r="F28">
+        <v>399550</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29">
+        <v>2010</v>
+      </c>
+      <c r="C29">
+        <v>177</v>
+      </c>
+      <c r="D29">
+        <v>993</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>26180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30">
+        <v>2009</v>
+      </c>
+      <c r="C30">
+        <v>2234</v>
+      </c>
+      <c r="D30">
+        <v>15754</v>
+      </c>
+      <c r="E30">
+        <v>21</v>
+      </c>
+      <c r="F30">
+        <v>367510</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31">
+        <v>2009</v>
+      </c>
+      <c r="C31">
+        <v>596</v>
+      </c>
+      <c r="D31">
+        <v>4530</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>112430</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32">
+        <v>2009</v>
+      </c>
+      <c r="C32">
+        <v>871</v>
+      </c>
+      <c r="D32">
+        <v>6453</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>148580</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33">
+        <v>2009</v>
+      </c>
+      <c r="C33">
+        <v>1896</v>
+      </c>
+      <c r="D33">
+        <v>14718</v>
+      </c>
+      <c r="E33">
+        <v>52</v>
+      </c>
+      <c r="F33">
+        <v>361815</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34">
+        <v>2009</v>
+      </c>
+      <c r="C34">
+        <v>1526</v>
+      </c>
+      <c r="D34">
+        <v>11543</v>
+      </c>
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34">
+        <v>290047</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35">
+        <v>2009</v>
+      </c>
+      <c r="C35">
+        <v>2976</v>
+      </c>
+      <c r="D35">
+        <v>19361</v>
+      </c>
+      <c r="E35">
+        <v>53</v>
+      </c>
+      <c r="F35">
+        <v>539630</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36">
+        <v>2009</v>
+      </c>
+      <c r="C36">
+        <v>5923</v>
+      </c>
+      <c r="D36">
+        <v>46345</v>
+      </c>
+      <c r="E36">
+        <v>203</v>
+      </c>
+      <c r="F36">
+        <v>1194675</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37">
+        <v>2009</v>
+      </c>
+      <c r="C37">
+        <v>1688</v>
+      </c>
+      <c r="D37">
+        <v>11470</v>
+      </c>
+      <c r="E37">
+        <v>28</v>
+      </c>
+      <c r="F37">
+        <v>309900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38">
+        <v>2009</v>
+      </c>
+      <c r="C38">
+        <v>3454</v>
+      </c>
+      <c r="D38">
+        <v>22794</v>
+      </c>
+      <c r="E38">
+        <v>54</v>
+      </c>
+      <c r="F38">
+        <v>561174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39">
+        <v>2009</v>
+      </c>
+      <c r="C39">
+        <v>4019</v>
+      </c>
+      <c r="D39">
+        <v>27506</v>
+      </c>
+      <c r="E39">
+        <v>215</v>
+      </c>
+      <c r="F39">
+        <v>817727</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40">
+        <v>2009</v>
+      </c>
+      <c r="C40">
+        <v>118</v>
+      </c>
+      <c r="D40">
+        <v>776</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>19890</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41">
+        <v>2009</v>
+      </c>
+      <c r="C41">
+        <v>114</v>
+      </c>
+      <c r="D41">
+        <v>792</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>21980</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42">
+        <v>2009</v>
+      </c>
+      <c r="C42">
+        <v>1771</v>
+      </c>
+      <c r="D42">
+        <v>16283</v>
+      </c>
+      <c r="E42">
+        <v>42</v>
+      </c>
+      <c r="F42">
+        <v>396942</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43">
+        <v>2009</v>
+      </c>
+      <c r="C43">
+        <v>181</v>
+      </c>
+      <c r="D43">
+        <v>939</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>26200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44">
+        <v>2008</v>
+      </c>
+      <c r="C44">
+        <v>2209</v>
+      </c>
+      <c r="D44">
+        <v>14764</v>
+      </c>
+      <c r="E44">
+        <v>19</v>
+      </c>
+      <c r="F44">
+        <v>367020</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45">
+        <v>2008</v>
+      </c>
+      <c r="C45">
+        <v>596</v>
+      </c>
+      <c r="D45">
+        <v>4295</v>
+      </c>
+      <c r="E45">
+        <v>11</v>
+      </c>
+      <c r="F45">
+        <v>111430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46">
+        <v>2008</v>
+      </c>
+      <c r="C46">
+        <v>884</v>
+      </c>
+      <c r="D46">
+        <v>6098</v>
+      </c>
+      <c r="E46">
+        <v>21</v>
+      </c>
+      <c r="F46">
+        <v>148300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47">
+        <v>2008</v>
+      </c>
+      <c r="C47">
+        <v>1826</v>
+      </c>
+      <c r="D47">
+        <v>14041</v>
+      </c>
+      <c r="E47">
+        <v>70</v>
+      </c>
+      <c r="F47">
+        <v>360428</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48">
+        <v>2008</v>
+      </c>
+      <c r="C48">
+        <v>1501</v>
+      </c>
+      <c r="D48">
+        <v>11153</v>
+      </c>
+      <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>288473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49">
+        <v>2008</v>
+      </c>
+      <c r="C49">
+        <v>2971</v>
+      </c>
+      <c r="D49">
+        <v>18048</v>
+      </c>
+      <c r="E49">
+        <v>126</v>
+      </c>
+      <c r="F49">
+        <v>535290</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50">
+        <v>2008</v>
+      </c>
+      <c r="C50">
+        <v>6348</v>
+      </c>
+      <c r="D50">
+        <v>45639</v>
+      </c>
+      <c r="E50">
+        <v>346</v>
+      </c>
+      <c r="F50">
+        <v>1192419</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>2008</v>
+      </c>
+      <c r="C51">
+        <v>1673</v>
+      </c>
+      <c r="D51">
+        <v>11131</v>
+      </c>
+      <c r="E51">
+        <v>38</v>
+      </c>
+      <c r="F51">
+        <v>308790</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52">
+        <v>2008</v>
+      </c>
+      <c r="C52">
+        <v>3415</v>
+      </c>
+      <c r="D52">
+        <v>21452</v>
+      </c>
+      <c r="E52">
+        <v>48</v>
+      </c>
+      <c r="F52">
+        <v>560042</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53">
+        <v>2008</v>
+      </c>
+      <c r="C53">
+        <v>3933</v>
+      </c>
+      <c r="D53">
+        <v>26240</v>
+      </c>
+      <c r="E53">
+        <v>221</v>
+      </c>
+      <c r="F53">
+        <v>809764</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54">
+        <v>2008</v>
+      </c>
+      <c r="C54">
+        <v>119</v>
+      </c>
+      <c r="D54">
+        <v>746</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>19860</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55">
+        <v>2008</v>
+      </c>
+      <c r="C55">
+        <v>115</v>
+      </c>
+      <c r="D55">
+        <v>752</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>21950</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56">
+        <v>2008</v>
+      </c>
+      <c r="C56">
+        <v>1692</v>
+      </c>
+      <c r="D56">
+        <v>15530</v>
+      </c>
+      <c r="E56">
+        <v>47</v>
+      </c>
+      <c r="F56">
+        <v>394134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57">
+        <v>2008</v>
+      </c>
+      <c r="C57">
+        <v>182</v>
+      </c>
+      <c r="D57">
+        <v>883</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>26300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58">
+        <v>2007</v>
+      </c>
+      <c r="C58">
+        <v>2235</v>
+      </c>
+      <c r="D58">
+        <v>13590</v>
+      </c>
+      <c r="E58">
+        <v>87</v>
+      </c>
+      <c r="F58">
+        <v>366450</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59">
+        <v>2007</v>
+      </c>
+      <c r="C59">
+        <v>578</v>
+      </c>
+      <c r="D59">
+        <v>3972</v>
+      </c>
+      <c r="E59">
+        <v>46</v>
+      </c>
+      <c r="F59">
+        <v>110247</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60">
+        <v>2007</v>
+      </c>
+      <c r="C60">
+        <v>913</v>
+      </c>
+      <c r="D60">
+        <v>5745</v>
+      </c>
+      <c r="E60">
+        <v>78</v>
+      </c>
+      <c r="F60">
+        <v>148030</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61">
+        <v>2007</v>
+      </c>
+      <c r="C61">
+        <v>1860</v>
+      </c>
+      <c r="D61">
+        <v>13291</v>
+      </c>
+      <c r="E61">
+        <v>220</v>
+      </c>
+      <c r="F61">
+        <v>358858</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62">
+        <v>2007</v>
+      </c>
+      <c r="C62">
+        <v>1519</v>
+      </c>
+      <c r="D62">
+        <v>10512</v>
+      </c>
+      <c r="E62">
+        <v>123</v>
+      </c>
+      <c r="F62">
+        <v>286053</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63">
+        <v>2007</v>
+      </c>
+      <c r="C63">
+        <v>2929</v>
+      </c>
+      <c r="D63">
+        <v>16873</v>
+      </c>
+      <c r="E63">
+        <v>820</v>
+      </c>
+      <c r="F63">
+        <v>529889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64">
+        <v>2007</v>
+      </c>
+      <c r="C64">
+        <v>5875</v>
+      </c>
+      <c r="D64">
+        <v>41928</v>
+      </c>
+      <c r="E64">
+        <v>495</v>
+      </c>
+      <c r="F64">
+        <v>1191584</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65">
+        <v>2007</v>
+      </c>
+      <c r="C65">
+        <v>1631</v>
+      </c>
+      <c r="D65">
+        <v>10212</v>
+      </c>
+      <c r="E65">
+        <v>102</v>
+      </c>
+      <c r="F65">
+        <v>306701</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>2007</v>
+      </c>
+      <c r="C66">
+        <v>3403</v>
+      </c>
+      <c r="D66">
+        <v>20287</v>
+      </c>
+      <c r="E66">
+        <v>149</v>
+      </c>
+      <c r="F66">
+        <v>558139</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67">
+        <v>2007</v>
+      </c>
+      <c r="C67">
+        <v>3990</v>
+      </c>
+      <c r="D67">
+        <v>25176</v>
+      </c>
+      <c r="E67">
+        <v>565</v>
+      </c>
+      <c r="F67">
+        <v>801310</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68">
+        <v>2007</v>
+      </c>
+      <c r="C68">
+        <v>115</v>
+      </c>
+      <c r="D68">
+        <v>703</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>19770</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69">
+        <v>2007</v>
+      </c>
+      <c r="C69">
+        <v>107</v>
+      </c>
+      <c r="D69">
+        <v>740</v>
+      </c>
+      <c r="E69">
+        <v>10</v>
+      </c>
+      <c r="F69">
+        <v>21880</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70">
+        <v>2007</v>
+      </c>
+      <c r="C70">
+        <v>1854</v>
+      </c>
+      <c r="D70">
+        <v>14484</v>
+      </c>
+      <c r="E70">
+        <v>279</v>
+      </c>
+      <c r="F70">
+        <v>391639</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71">
+        <v>2007</v>
+      </c>
+      <c r="C71">
+        <v>167</v>
+      </c>
+      <c r="D71">
+        <v>846</v>
+      </c>
+      <c r="E71">
+        <v>11</v>
+      </c>
+      <c r="F71">
+        <v>26350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
@@ -3785,7 +5233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5"/>

</xml_diff>